<commit_message>
updated preliminary analysis and table
</commit_message>
<xml_diff>
--- a/tables_figures/final_tables_figures/Tables.xlsx
+++ b/tables_figures/final_tables_figures/Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/11-DOC-ELA_animal-excretion/tables_figures/final_tables_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="781" documentId="8_{F2CF8D58-C965-49FA-B673-1C494D076C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{782B03C9-1841-4687-A5DA-3FA10F644117}"/>
+  <xr:revisionPtr revIDLastSave="787" documentId="8_{F2CF8D58-C965-49FA-B673-1C494D076C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F69D5941-AFCA-45F5-9525-CA7E2D4C7074}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0BA4557E-E60D-4DC8-8833-FFFA2208CF63}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="117">
   <si>
     <t>Lake</t>
   </si>
@@ -162,7 +162,26 @@
   </si>
   <si>
     <r>
-      <t>DOC (mg L</t>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (m</t>
     </r>
     <r>
       <rPr>
@@ -186,26 +205,7 @@
   </si>
   <si>
     <r>
-      <t>K</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>d</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> (m</t>
+      <t>Conductivity (µS cm</t>
     </r>
     <r>
       <rPr>
@@ -229,7 +229,7 @@
   </si>
   <si>
     <r>
-      <t>Conductivity (µS cm</t>
+      <t>TDP (µg P L</t>
     </r>
     <r>
       <rPr>
@@ -253,55 +253,7 @@
   </si>
   <si>
     <r>
-      <t>TDP (µg P L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>TDN (µg N L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Epilimnetic chl-a (µg L</t>
     </r>
     <r>
       <rPr>
@@ -921,18 +873,34 @@
   </si>
   <si>
     <r>
-      <t>Lake surface area (Area), mean depth (Z</t>
+      <t xml:space="preserve">lnRR N ~ </t>
     </r>
     <r>
       <rPr>
         <i/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>mean</t>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(DOC)</t>
+    </r>
+  </si>
+  <si>
+    <t>lnRR N ~ 1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">lnRR P ~ </t>
     </r>
     <r>
       <rPr>
@@ -942,42 +910,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>), max depth (Z</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>max</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>), and water retention time (WRT)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">lnRR N ~ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>f</t>
     </r>
     <r>
@@ -991,20 +923,16 @@
     </r>
   </si>
   <si>
-    <t>lnRR N ~ 1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">lnRR P ~ </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
+    <t>lnRR P ~ 1</t>
+  </si>
+  <si>
+    <t>lnRR N</t>
+  </si>
+  <si>
+    <t>lnRR P</t>
+  </si>
+  <si>
+    <r>
       <t>f</t>
     </r>
     <r>
@@ -1018,26 +946,51 @@
     </r>
   </si>
   <si>
-    <t>lnRR P ~ 1</t>
-  </si>
-  <si>
-    <t>lnRR N</t>
-  </si>
-  <si>
-    <t>lnRR P</t>
-  </si>
-  <si>
-    <r>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(DOC)</t>
+    <r>
+      <t>Chl-a (µg L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DOC (mg C L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
 </sst>
@@ -1049,7 +1002,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1109,14 +1062,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <vertAlign val="subscript"/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2613,10 +2558,14 @@
 </externalLink>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2654,7 +2603,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2760,7 +2709,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2902,7 +2851,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2913,7 +2862,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N13"/>
+      <selection activeCell="M7" sqref="M6:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2921,12 +2870,12 @@
     <col min="2" max="2" width="7.81640625" customWidth="1"/>
     <col min="3" max="3" width="7.453125" customWidth="1"/>
     <col min="4" max="5" width="6.1796875" customWidth="1"/>
-    <col min="7" max="7" width="7.36328125" customWidth="1"/>
-    <col min="8" max="8" width="13.6328125" customWidth="1"/>
-    <col min="9" max="9" width="13.90625" customWidth="1"/>
-    <col min="10" max="10" width="8" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" customWidth="1"/>
-    <col min="12" max="12" width="9.08984375" customWidth="1"/>
+    <col min="6" max="6" width="7.36328125" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="11" max="11" width="9.08984375" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" customWidth="1"/>
     <col min="13" max="13" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2944,31 +2893,31 @@
         <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>3</v>
@@ -2990,33 +2939,33 @@
       <c r="E2" s="3">
         <v>1.24</v>
       </c>
-      <c r="F2" s="4">
-        <v>6.335</v>
+      <c r="F2" s="5">
+        <v>0.80700000000000005</v>
       </c>
       <c r="G2" s="5">
-        <v>0.80700000000000005</v>
-      </c>
-      <c r="H2" s="5">
         <v>3.38</v>
       </c>
-      <c r="I2" s="3">
+      <c r="H2" s="3">
         <f>AVERAGE('[1]2022_RBR_Conductivity'!$D$16:$D$31)</f>
         <v>11.084375</v>
       </c>
-      <c r="J2" s="3">
+      <c r="I2" s="3">
         <v>6.08</v>
       </c>
+      <c r="J2" s="4">
+        <v>6.335</v>
+      </c>
       <c r="K2" s="5">
+        <v>283</v>
+      </c>
+      <c r="L2" s="5">
         <v>2.7</v>
-      </c>
-      <c r="L2" s="5">
-        <v>283</v>
       </c>
       <c r="M2" s="5">
         <v>3.79</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -3037,31 +2986,31 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="F3" s="5">
+        <v>1.296</v>
+      </c>
+      <c r="G3" s="5">
+        <v>2.25</v>
+      </c>
+      <c r="H3" s="3">
+        <v>21.88</v>
+      </c>
+      <c r="I3" s="3">
+        <v>6.6</v>
+      </c>
+      <c r="J3" s="5">
         <v>10.039999999999999</v>
       </c>
-      <c r="G3" s="5">
-        <v>1.296</v>
-      </c>
-      <c r="H3" s="5">
-        <v>2.25</v>
-      </c>
-      <c r="I3" s="3">
-        <v>21.88</v>
-      </c>
-      <c r="J3" s="3">
-        <v>6.6</v>
-      </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="5">
+        <v>349</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="L3" s="5">
-        <v>349</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -3080,33 +3029,33 @@
       <c r="E4" s="3">
         <v>13.42</v>
       </c>
-      <c r="F4" s="3">
-        <v>3.4620000000000002</v>
+      <c r="F4" s="5">
+        <v>0.433</v>
       </c>
       <c r="G4" s="5">
-        <v>0.433</v>
-      </c>
-      <c r="H4" s="5">
         <v>4.38</v>
       </c>
-      <c r="I4" s="3">
+      <c r="H4" s="3">
         <f>AVERAGE('[1]2022_RBR_Conductivity'!$D$195:$D$233)</f>
         <v>12.023589743589747</v>
       </c>
+      <c r="I4" s="3">
+        <v>5.85</v>
+      </c>
       <c r="J4" s="3">
-        <v>5.85</v>
+        <v>3.4620000000000002</v>
       </c>
       <c r="K4" s="5">
+        <v>184</v>
+      </c>
+      <c r="L4" s="5">
         <v>1.4</v>
-      </c>
-      <c r="L4" s="5">
-        <v>184</v>
       </c>
       <c r="M4" s="5">
         <v>1.17</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -3125,33 +3074,33 @@
       <c r="E5" s="3">
         <v>6.65</v>
       </c>
-      <c r="F5" s="3">
-        <v>7.1559999999999997</v>
+      <c r="F5" s="5">
+        <v>0.82599999999999996</v>
       </c>
       <c r="G5" s="5">
-        <v>0.82599999999999996</v>
-      </c>
-      <c r="H5" s="5">
         <v>4.38</v>
       </c>
-      <c r="I5" s="3">
+      <c r="H5" s="3">
         <f>AVERAGE('[1]2022_RBR_Conductivity'!$D$603:$D$644)</f>
         <v>17.215476190476188</v>
       </c>
+      <c r="I5" s="3">
+        <v>6.61</v>
+      </c>
       <c r="J5" s="3">
-        <v>6.61</v>
+        <v>7.1559999999999997</v>
       </c>
       <c r="K5" s="5">
+        <v>290</v>
+      </c>
+      <c r="L5" s="5">
         <v>5.4</v>
-      </c>
-      <c r="L5" s="5">
-        <v>290</v>
       </c>
       <c r="M5" s="5">
         <v>2.96</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -3170,33 +3119,33 @@
       <c r="E6" s="3">
         <v>16.03</v>
       </c>
-      <c r="F6" s="3">
-        <v>3.9550000000000001</v>
+      <c r="F6" s="5">
+        <v>0.45300000000000001</v>
       </c>
       <c r="G6" s="5">
-        <v>0.45300000000000001</v>
-      </c>
-      <c r="H6" s="5">
         <v>3.63</v>
       </c>
-      <c r="I6" s="3">
+      <c r="H6" s="3">
         <f>AVERAGE('[1]2022_RBR_Conductivity'!$D$1116:$D$1145)</f>
         <v>18.313333333333333</v>
       </c>
+      <c r="I6" s="3">
+        <v>6.05</v>
+      </c>
       <c r="J6" s="3">
-        <v>6.05</v>
+        <v>3.9550000000000001</v>
       </c>
       <c r="K6" s="5">
+        <v>217</v>
+      </c>
+      <c r="L6" s="5">
         <v>1.8</v>
-      </c>
-      <c r="L6" s="5">
-        <v>217</v>
       </c>
       <c r="M6" s="5">
         <v>1.1499999999999999</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -3215,33 +3164,33 @@
       <c r="E7" s="3">
         <v>5.13</v>
       </c>
-      <c r="F7" s="3">
-        <v>5.6909999999999998</v>
+      <c r="F7" s="5">
+        <v>0.52900000000000003</v>
       </c>
       <c r="G7" s="5">
-        <v>0.52900000000000003</v>
-      </c>
-      <c r="H7" s="5">
         <v>3.63</v>
       </c>
-      <c r="I7" s="3">
+      <c r="H7" s="3">
         <f>AVERAGE('[1]2022_RBR_Conductivity'!$D$1475:$D$1514)</f>
         <v>30.526000000000003</v>
       </c>
+      <c r="I7" s="3">
+        <v>6.07</v>
+      </c>
       <c r="J7" s="3">
-        <v>6.07</v>
+        <v>5.6909999999999998</v>
       </c>
       <c r="K7" s="5">
+        <v>205</v>
+      </c>
+      <c r="L7" s="5">
         <v>4.5</v>
-      </c>
-      <c r="L7" s="5">
-        <v>205</v>
       </c>
       <c r="M7" s="5">
         <v>0.87</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -3260,33 +3209,33 @@
       <c r="E8" s="3">
         <v>0.43</v>
       </c>
-      <c r="F8" s="3">
-        <v>5.26</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="F8" s="5">
         <v>0.55500000000000005</v>
       </c>
-      <c r="H8" s="3">
+      <c r="G8" s="3">
         <f>AVERAGE(6.38, 5.63)</f>
         <v>6.0049999999999999</v>
       </c>
+      <c r="H8" s="3">
+        <v>17.57</v>
+      </c>
       <c r="I8" s="3">
-        <v>17.57</v>
+        <v>6.49</v>
       </c>
       <c r="J8" s="3">
-        <v>6.49</v>
+        <v>5.26</v>
       </c>
       <c r="K8" s="5">
+        <v>234</v>
+      </c>
+      <c r="L8" s="5">
         <v>3.5</v>
-      </c>
-      <c r="L8" s="5">
-        <v>234</v>
       </c>
       <c r="M8" s="5">
         <v>1.3</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -3305,33 +3254,33 @@
       <c r="E9" s="3">
         <v>6.22</v>
       </c>
-      <c r="F9" s="3">
-        <v>7.2439999999999998</v>
+      <c r="F9" s="5">
+        <v>0.65500000000000003</v>
       </c>
       <c r="G9" s="5">
-        <v>0.65500000000000003</v>
-      </c>
-      <c r="H9" s="5">
         <v>3.38</v>
       </c>
-      <c r="I9" s="3">
+      <c r="H9" s="3">
         <f>AVERAGE('[1]2022_RBR_Conductivity'!$D$1753:$D$1784)</f>
         <v>14.975000000000001</v>
       </c>
+      <c r="I9" s="3">
+        <v>5.91</v>
+      </c>
       <c r="J9" s="3">
-        <v>5.91</v>
+        <v>7.2439999999999998</v>
       </c>
       <c r="K9" s="5">
+        <v>256</v>
+      </c>
+      <c r="L9" s="5">
         <v>3.8</v>
-      </c>
-      <c r="L9" s="5">
-        <v>256</v>
       </c>
       <c r="M9" s="5">
         <v>2.0099999999999998</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -3350,33 +3299,33 @@
       <c r="E10" s="3">
         <v>3.51</v>
       </c>
-      <c r="F10" s="3">
-        <v>6.8129999999999997</v>
+      <c r="F10" s="5">
+        <v>0.64300000000000002</v>
       </c>
       <c r="G10" s="5">
-        <v>0.64300000000000002</v>
-      </c>
-      <c r="H10" s="5">
         <v>2.88</v>
       </c>
-      <c r="I10" s="3">
+      <c r="H10" s="3">
         <f>AVERAGE('[1]2022_RBR_Conductivity'!$D$2042:$D$2070)</f>
         <v>15.971379310344831</v>
       </c>
+      <c r="I10" s="3">
+        <v>6.49</v>
+      </c>
       <c r="J10" s="3">
-        <v>6.49</v>
+        <v>6.8129999999999997</v>
       </c>
       <c r="K10" s="5">
+        <v>258</v>
+      </c>
+      <c r="L10" s="5">
         <v>0.7</v>
-      </c>
-      <c r="L10" s="5">
-        <v>258</v>
       </c>
       <c r="M10" s="5">
         <v>1.45</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -3396,32 +3345,32 @@
       <c r="E11" s="3">
         <v>0.1</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="6">
+        <v>0.84</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="I11" s="3">
+        <v>7.21</v>
+      </c>
+      <c r="J11" s="3">
         <v>10.91</v>
       </c>
-      <c r="G11" s="6">
-        <v>0.84</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="3">
-        <v>12.4</v>
-      </c>
-      <c r="J11" s="3">
-        <v>7.21</v>
-      </c>
-      <c r="K11" s="5">
+      <c r="K11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="5">
         <v>5.6</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -3440,39 +3389,37 @@
       <c r="E12" s="8">
         <v>2.09</v>
       </c>
-      <c r="F12" s="8">
-        <v>5.0579999999999998</v>
+      <c r="F12" s="9">
+        <v>0.503</v>
       </c>
       <c r="G12" s="9">
-        <v>0.503</v>
-      </c>
-      <c r="H12" s="9">
         <v>3.13</v>
       </c>
-      <c r="I12" s="8">
+      <c r="H12" s="8">
         <f>AVERAGE('[1]2022_RBR_Conductivity'!$D$2331:$D$2364)</f>
         <v>14.551764705882354</v>
       </c>
+      <c r="I12" s="8">
+        <v>6.51</v>
+      </c>
       <c r="J12" s="8">
-        <v>6.51</v>
+        <v>5.0579999999999998</v>
       </c>
       <c r="K12" s="9">
+        <v>296</v>
+      </c>
+      <c r="L12" s="9">
         <v>4.7</v>
-      </c>
-      <c r="L12" s="9">
-        <v>296</v>
       </c>
       <c r="M12" s="9">
         <v>1.37</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="25" t="s">
-        <v>110</v>
-      </c>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3496,33 +3443,33 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>79</v>
-      </c>
       <c r="F1" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" s="18">
         <v>353</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D2" s="30">
         <v>4.2620392137853598</v>
@@ -3539,13 +3486,13 @@
     </row>
     <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" s="18">
         <v>353</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D3" s="30">
         <v>1.8475515119346599</v>
@@ -3562,13 +3509,13 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="18">
         <v>353</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4" s="30">
         <v>0.18802276820660199</v>
@@ -3584,13 +3531,13 @@
     </row>
     <row r="5" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="18">
         <v>77</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" s="32">
         <v>0</v>
@@ -3606,13 +3553,13 @@
     </row>
     <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="18">
         <v>77</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6" s="32">
         <v>0</v>
@@ -3627,13 +3574,13 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="18">
         <v>77</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D7" s="32">
         <v>0</v>
@@ -3649,13 +3596,13 @@
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B8" s="19">
         <v>353</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D8" s="34">
         <v>0.17249999999999999</v>
@@ -3672,7 +3619,7 @@
     </row>
     <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -3695,21 +3642,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>31</v>
-      </c>
       <c r="D1" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2">
         <v>12</v>
@@ -3724,7 +3671,7 @@
     </row>
     <row r="3" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2">
         <v>14</v>
@@ -3739,7 +3686,7 @@
     </row>
     <row r="4" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -3754,7 +3701,7 @@
     </row>
     <row r="5" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2">
         <v>9</v>
@@ -3769,7 +3716,7 @@
     </row>
     <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2">
         <v>14</v>
@@ -3784,7 +3731,7 @@
     </row>
     <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
@@ -3799,7 +3746,7 @@
     </row>
     <row r="8" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2">
         <v>9</v>
@@ -3814,7 +3761,7 @@
     </row>
     <row r="9" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2">
         <v>12</v>
@@ -3829,7 +3776,7 @@
     </row>
     <row r="10" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2">
         <v>3</v>
@@ -3844,7 +3791,7 @@
     </row>
     <row r="11" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B11" s="2">
         <v>7</v>
@@ -3859,7 +3806,7 @@
     </row>
     <row r="12" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B12" s="2">
         <v>2</v>
@@ -3874,7 +3821,7 @@
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B13" s="2">
         <v>3</v>
@@ -3889,7 +3836,7 @@
     </row>
     <row r="14" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B14" s="7">
         <v>2</v>
@@ -3922,10 +3869,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
@@ -3933,18 +3880,18 @@
     <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
       <c r="B2" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -3952,7 +3899,7 @@
     </row>
     <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" s="18">
         <v>3.5840000000000001</v>
@@ -3966,7 +3913,7 @@
     </row>
     <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="18">
         <v>3.8780000000000001</v>
@@ -3980,13 +3927,13 @@
     </row>
     <row r="6" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="38">
         <v>0.02</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" s="38">
         <v>0.01</v>
@@ -3994,14 +3941,14 @@
     </row>
     <row r="7" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
     <row r="8" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" s="18">
         <v>3.6480000000000001</v>
@@ -4015,7 +3962,7 @@
     </row>
     <row r="9" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B9" s="18">
         <v>3.964</v>
@@ -4029,21 +3976,21 @@
     </row>
     <row r="10" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" s="38">
         <v>0.03</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B11" s="18">
         <v>4.4960000000000004</v>
@@ -4057,7 +4004,7 @@
     </row>
     <row r="12" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B12" s="18">
         <v>0.24</v>
@@ -4071,7 +4018,7 @@
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B13" s="19">
         <v>28</v>
@@ -4085,7 +4032,7 @@
     </row>
     <row r="14" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -4118,36 +4065,36 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="F1" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2">
         <v>77</v>
@@ -4164,13 +4111,13 @@
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" s="2">
         <v>77</v>
@@ -4187,13 +4134,13 @@
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" s="2">
         <v>77</v>
@@ -4210,13 +4157,13 @@
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" s="2">
         <v>77</v>
@@ -4233,13 +4180,13 @@
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" s="2">
         <v>77</v>
@@ -4256,13 +4203,13 @@
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="2">
         <v>77</v>
@@ -4279,13 +4226,13 @@
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="2">
         <v>77</v>
@@ -4302,13 +4249,13 @@
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="2">
         <v>77</v>
@@ -4325,13 +4272,13 @@
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="2">
         <v>77</v>
@@ -4348,13 +4295,13 @@
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11" s="2">
         <v>77</v>
@@ -4371,13 +4318,13 @@
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12" s="7">
         <v>77</v>
@@ -4413,39 +4360,39 @@
   <sheetData>
     <row r="1" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -4465,13 +4412,13 @@
     </row>
     <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -4491,13 +4438,13 @@
     </row>
     <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -4517,13 +4464,13 @@
     </row>
     <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -4543,13 +4490,13 @@
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -4569,13 +4516,13 @@
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -4595,13 +4542,13 @@
     </row>
     <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -4621,13 +4568,13 @@
     </row>
     <row r="9" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -4647,13 +4594,13 @@
     </row>
     <row r="10" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -4673,13 +4620,13 @@
     </row>
     <row r="11" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -4699,13 +4646,13 @@
     </row>
     <row r="12" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -4725,13 +4672,13 @@
     </row>
     <row r="13" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -4751,13 +4698,13 @@
     </row>
     <row r="14" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
@@ -4777,13 +4724,13 @@
     </row>
     <row r="15" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -4803,13 +4750,13 @@
     </row>
     <row r="16" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
@@ -4829,13 +4776,13 @@
     </row>
     <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -4855,13 +4802,13 @@
     </row>
     <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2">
         <v>0</v>
@@ -4881,13 +4828,13 @@
     </row>
     <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -4907,13 +4854,13 @@
     </row>
     <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D20" s="2">
         <v>0</v>
@@ -4933,13 +4880,13 @@
     </row>
     <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
@@ -4959,13 +4906,13 @@
     </row>
     <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -4985,13 +4932,13 @@
     </row>
     <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -5011,13 +4958,13 @@
     </row>
     <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D24" s="2">
         <v>0</v>
@@ -5037,13 +4984,13 @@
     </row>
     <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -5063,13 +5010,13 @@
     </row>
     <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -5089,13 +5036,13 @@
     </row>
     <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
@@ -5115,13 +5062,13 @@
     </row>
     <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
@@ -5141,13 +5088,13 @@
     </row>
     <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D29" s="2">
         <v>0</v>
@@ -5167,13 +5114,13 @@
     </row>
     <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
@@ -5193,13 +5140,13 @@
     </row>
     <row r="31" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -5219,13 +5166,13 @@
     </row>
     <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D32" s="2">
         <v>0</v>
@@ -5245,13 +5192,13 @@
     </row>
     <row r="33" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -5271,13 +5218,13 @@
     </row>
     <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D34" s="7">
         <v>0</v>
@@ -5312,32 +5259,32 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
       <c r="B2" s="22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" s="18">
         <v>4.2619999999999996</v>
@@ -5348,7 +5295,7 @@
     </row>
     <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" s="18">
         <v>4.9859999999999998</v>
@@ -5359,7 +5306,7 @@
     </row>
     <row r="6" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="18">
         <v>0.01</v>
@@ -5370,7 +5317,7 @@
     </row>
     <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="18">
         <v>0.06</v>
@@ -5381,7 +5328,7 @@
     </row>
     <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B8" s="18">
         <v>0.79</v>
@@ -5392,7 +5339,7 @@
     </row>
     <row r="9" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B9" s="19">
         <v>88</v>

</xml_diff>

<commit_message>
updated figures and tested new models
</commit_message>
<xml_diff>
--- a/tables_figures/final_tables_figures/Tables.xlsx
+++ b/tables_figures/final_tables_figures/Tables.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/11-DOC-ELA_animal-excretion/tables_figures/final_tables_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="903" documentId="8_{F2CF8D58-C965-49FA-B673-1C494D076C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF40F436-0959-4B31-986B-43F42E7A141D}"/>
+  <xr:revisionPtr revIDLastSave="1178" documentId="8_{F2CF8D58-C965-49FA-B673-1C494D076C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D66B8AF-64BA-492D-97B9-92CF56C03106}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="37140" yWindow="1710" windowWidth="14445" windowHeight="7305" activeTab="6" xr2:uid="{0BA4557E-E60D-4DC8-8833-FFFA2208CF63}"/>
+    <workbookView minimized="1" xWindow="2380" yWindow="1180" windowWidth="14400" windowHeight="7280" activeTab="1" xr2:uid="{0BA4557E-E60D-4DC8-8833-FFFA2208CF63}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table S1" sheetId="3" r:id="rId2"/>
-    <sheet name="Table S2" sheetId="2" r:id="rId3"/>
-    <sheet name="Table S3" sheetId="6" r:id="rId4"/>
-    <sheet name="Table S4" sheetId="5" r:id="rId5"/>
-    <sheet name="Table S5" sheetId="4" r:id="rId6"/>
-    <sheet name="Table S6" sheetId="7" r:id="rId7"/>
+    <sheet name="Table 2" sheetId="8" r:id="rId2"/>
+    <sheet name="Table S1" sheetId="3" r:id="rId3"/>
+    <sheet name="Table S2" sheetId="2" r:id="rId4"/>
+    <sheet name="Table S3" sheetId="6" r:id="rId5"/>
+    <sheet name="Table S4" sheetId="5" r:id="rId6"/>
+    <sheet name="Table S5" sheetId="4" r:id="rId7"/>
+    <sheet name="Table S6" sheetId="7" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Table1!$A$1:$N$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Table1!$A$1:$I$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="134">
   <si>
     <t>Lake</t>
   </si>
@@ -640,30 +641,6 @@
   </si>
   <si>
     <t>null model</t>
-  </si>
-  <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>YP</t>
-  </si>
-  <si>
-    <t>FM, WS, PD</t>
-  </si>
-  <si>
-    <t>WS, PD</t>
-  </si>
-  <si>
-    <t>FM, WS, PD, YP</t>
-  </si>
-  <si>
-    <t>WS, PD, YP</t>
-  </si>
-  <si>
-    <t>PD, YP</t>
-  </si>
-  <si>
-    <t>FM, WS</t>
   </si>
   <si>
     <t>mean (± SD)</t>
@@ -948,17 +925,594 @@
   </si>
   <si>
     <t>medium</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LH, LT, NP, WS, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>YP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, SS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LT, NRD, FD, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NPD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>WS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, SS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LT, WS, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>YP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, SS, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NPD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, LC, FD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SUVA</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">254 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(L mg-1 C m-1)</t>
+    </r>
+  </si>
+  <si>
+    <t>FI (unitless)</t>
+  </si>
+  <si>
+    <t>C2 (RU)</t>
+  </si>
+  <si>
+    <t>C5 (RU)</t>
+  </si>
+  <si>
+    <t>C7 (RU)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NP, BnS, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>YP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LT, LC, BnS, StS, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NPD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>WS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, B, BS, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>YP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, SS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LT, NRD, BnS, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FhM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NPD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>WS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, BS, SS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NRD, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FhM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, NPD, WS, ID</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NRD, FD, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FhM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, PD, BS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LT, LC, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FhM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NPD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>WS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LT, NRD, FD, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FhM,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NPD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>WS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, SS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LH, LT, LC, BnS, StS, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FhM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, LgD, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>NPD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>WS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, B, BS, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>YP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Fish species abbreviations as follows: LT, Lake trout (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Salvelinus namaycush</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>); NP, Northern pike (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Esox lucius</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">); </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B, Burbot (Lota lota); WS, White sucker (Catostomus commersoni); SS, Slimy sculpin (Cottus cognatus); BS, Brook stickleback (Culaea inconstans); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRD, Northern redbelly dace (Chrosomus eos);  FD, Finescale dace (Chrosomus neogaeus); ID, Iowa darter (Etheostoma exile);  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPD, Northern pearl dace (Margariscus nachtriebi); BnS, Blacknose shiner (Notripis heterolepis);  StS, Spottail shiner (Notropis hudsonius); </t>
+  </si>
+  <si>
+    <t>YP, Yellow perch (Perca flaescens); FhM, Fathead minnow (Pimephales promelas);  LgD, Longnose dace (Rhinichthys cataractae);</t>
+  </si>
+  <si>
+    <t>LC, Lake chub (Couesius plumbeus); LH, Lake herring (Coregonus artedi)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1019,6 +1573,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1069,7 +1642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1082,9 +1655,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1167,17 +1737,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1193,17 +1759,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2846,10 +3419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD1C4D6-4894-4E08-BEFA-8BF0F75F7B5F}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A12"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2861,12 +3434,9 @@
     <col min="7" max="7" width="13.6328125" customWidth="1"/>
     <col min="8" max="8" width="13.90625" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="11" max="11" width="9.08984375" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" customWidth="1"/>
-    <col min="13" max="13" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="52.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="38" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2880,7 +3450,7 @@
         <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>23</v>
@@ -2894,23 +3464,8 @@
       <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2926,7 +3481,7 @@
       <c r="E2" s="3">
         <v>1.24</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <v>0.80700000000000005</v>
       </c>
       <c r="G2" s="5">
@@ -2939,23 +3494,8 @@
       <c r="I2" s="3">
         <v>6.08</v>
       </c>
-      <c r="J2" s="4">
-        <v>6.335</v>
-      </c>
-      <c r="K2" s="5">
-        <v>283</v>
-      </c>
-      <c r="L2" s="5">
-        <v>2.7</v>
-      </c>
-      <c r="M2" s="5">
-        <v>3.79</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -2972,7 +3512,7 @@
       <c r="E3" s="3">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>1.296</v>
       </c>
       <c r="G3" s="5">
@@ -2984,23 +3524,8 @@
       <c r="I3" s="3">
         <v>6.6</v>
       </c>
-      <c r="J3" s="5">
-        <v>10.039999999999999</v>
-      </c>
-      <c r="K3" s="5">
-        <v>349</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3016,7 +3541,7 @@
       <c r="E4" s="3">
         <v>13.42</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>0.433</v>
       </c>
       <c r="G4" s="5">
@@ -3029,23 +3554,8 @@
       <c r="I4" s="3">
         <v>5.85</v>
       </c>
-      <c r="J4" s="3">
-        <v>3.4620000000000002</v>
-      </c>
-      <c r="K4" s="5">
-        <v>184</v>
-      </c>
-      <c r="L4" s="5">
-        <v>1.4</v>
-      </c>
-      <c r="M4" s="5">
-        <v>1.17</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3061,7 +3571,7 @@
       <c r="E5" s="3">
         <v>6.65</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>0.82599999999999996</v>
       </c>
       <c r="G5" s="5">
@@ -3074,23 +3584,8 @@
       <c r="I5" s="3">
         <v>6.61</v>
       </c>
-      <c r="J5" s="3">
-        <v>7.1559999999999997</v>
-      </c>
-      <c r="K5" s="5">
-        <v>290</v>
-      </c>
-      <c r="L5" s="5">
-        <v>5.4</v>
-      </c>
-      <c r="M5" s="5">
-        <v>2.96</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -3106,7 +3601,7 @@
       <c r="E6" s="3">
         <v>16.03</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>0.45300000000000001</v>
       </c>
       <c r="G6" s="5">
@@ -3119,23 +3614,8 @@
       <c r="I6" s="3">
         <v>6.05</v>
       </c>
-      <c r="J6" s="3">
-        <v>3.9550000000000001</v>
-      </c>
-      <c r="K6" s="5">
-        <v>217</v>
-      </c>
-      <c r="L6" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="M6" s="5">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -3151,7 +3631,7 @@
       <c r="E7" s="3">
         <v>5.13</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>0.52900000000000003</v>
       </c>
       <c r="G7" s="5">
@@ -3164,23 +3644,8 @@
       <c r="I7" s="3">
         <v>6.07</v>
       </c>
-      <c r="J7" s="3">
-        <v>5.6909999999999998</v>
-      </c>
-      <c r="K7" s="5">
-        <v>205</v>
-      </c>
-      <c r="L7" s="5">
-        <v>4.5</v>
-      </c>
-      <c r="M7" s="5">
-        <v>0.87</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -3196,7 +3661,7 @@
       <c r="E8" s="3">
         <v>0.43</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>0.55500000000000005</v>
       </c>
       <c r="G8" s="3">
@@ -3209,23 +3674,8 @@
       <c r="I8" s="3">
         <v>6.49</v>
       </c>
-      <c r="J8" s="3">
-        <v>5.26</v>
-      </c>
-      <c r="K8" s="5">
-        <v>234</v>
-      </c>
-      <c r="L8" s="5">
-        <v>3.5</v>
-      </c>
-      <c r="M8" s="5">
-        <v>1.3</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3241,7 +3691,7 @@
       <c r="E9" s="3">
         <v>6.22</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>0.65500000000000003</v>
       </c>
       <c r="G9" s="5">
@@ -3254,23 +3704,8 @@
       <c r="I9" s="3">
         <v>5.91</v>
       </c>
-      <c r="J9" s="3">
-        <v>7.2439999999999998</v>
-      </c>
-      <c r="K9" s="5">
-        <v>256</v>
-      </c>
-      <c r="L9" s="5">
-        <v>3.8</v>
-      </c>
-      <c r="M9" s="5">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -3286,7 +3721,7 @@
       <c r="E10" s="3">
         <v>3.51</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>0.64300000000000002</v>
       </c>
       <c r="G10" s="5">
@@ -3299,23 +3734,8 @@
       <c r="I10" s="3">
         <v>6.49</v>
       </c>
-      <c r="J10" s="3">
-        <v>6.8129999999999997</v>
-      </c>
-      <c r="K10" s="5">
-        <v>258</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="M10" s="5">
-        <v>1.45</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -3332,7 +3752,7 @@
       <c r="E11" s="3">
         <v>0.1</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="3">
         <v>0.84</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -3344,69 +3764,39 @@
       <c r="I11" s="3">
         <v>7.21</v>
       </c>
-      <c r="J11" s="3">
-        <v>10.91</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="5">
-        <v>5.6</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+    </row>
+    <row r="12" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>26.132999999999999</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>7.27</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>13.11</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>2.09</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>0.503</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>3.13</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <f>AVERAGE('[1]2022_RBR_Conductivity'!$D$2331:$D$2364)</f>
         <v>14.551764705882354</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <v>6.51</v>
       </c>
-      <c r="J12" s="8">
-        <v>5.0579999999999998</v>
-      </c>
-      <c r="K12" s="9">
-        <v>296</v>
-      </c>
-      <c r="L12" s="9">
-        <v>4.7</v>
-      </c>
-      <c r="M12" s="9">
-        <v>1.37</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="25"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3414,6 +3804,476 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C82D021-8F4C-4E71-986C-08A9033EF321}">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A1:K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4">
+        <v>6.335</v>
+      </c>
+      <c r="C2" s="51">
+        <v>2.5188978660000001</v>
+      </c>
+      <c r="D2" s="51">
+        <v>1.259755832</v>
+      </c>
+      <c r="E2" s="51">
+        <v>0.73122500000000001</v>
+      </c>
+      <c r="F2" s="51">
+        <v>0.14449489400000001</v>
+      </c>
+      <c r="G2" s="51">
+        <v>0.27149173799999998</v>
+      </c>
+      <c r="H2" s="5">
+        <v>283</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="J2" s="5">
+        <v>3.79</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="31" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5">
+        <v>10.039999999999999</v>
+      </c>
+      <c r="C3" s="51">
+        <v>3.8440824120000001</v>
+      </c>
+      <c r="D3" s="51">
+        <v>1.284469147</v>
+      </c>
+      <c r="E3" s="51">
+        <v>1.4567019729999999</v>
+      </c>
+      <c r="F3" s="51">
+        <v>0.29113379499999997</v>
+      </c>
+      <c r="G3" s="51">
+        <v>0.21290036500000001</v>
+      </c>
+      <c r="H3" s="5">
+        <v>349</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3.4620000000000002</v>
+      </c>
+      <c r="C4" s="51">
+        <v>1.913706441</v>
+      </c>
+      <c r="D4" s="51">
+        <v>1.2597043109999999</v>
+      </c>
+      <c r="E4" s="51">
+        <v>0.17739898100000001</v>
+      </c>
+      <c r="F4" s="51">
+        <v>2.9624553000000001E-2</v>
+      </c>
+      <c r="G4" s="51">
+        <v>0.15317287199999999</v>
+      </c>
+      <c r="H4" s="5">
+        <v>184</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1.17</v>
+      </c>
+      <c r="K4" s="36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>7.1559999999999997</v>
+      </c>
+      <c r="C5" s="51">
+        <v>3.2496000939999998</v>
+      </c>
+      <c r="D5" s="51">
+        <v>1.2246417000000001</v>
+      </c>
+      <c r="E5" s="51">
+        <v>1.204860883</v>
+      </c>
+      <c r="F5" s="51">
+        <v>0.13577767499999999</v>
+      </c>
+      <c r="G5" s="51">
+        <v>0.21650597999999999</v>
+      </c>
+      <c r="H5" s="5">
+        <v>290</v>
+      </c>
+      <c r="I5" s="5">
+        <v>5.4</v>
+      </c>
+      <c r="J5" s="5">
+        <v>2.96</v>
+      </c>
+      <c r="K5" s="36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3.9550000000000001</v>
+      </c>
+      <c r="C6" s="51">
+        <v>1.794215745</v>
+      </c>
+      <c r="D6" s="51">
+        <v>1.3143496750000001</v>
+      </c>
+      <c r="E6" s="51">
+        <v>0.19550811500000001</v>
+      </c>
+      <c r="F6" s="51">
+        <v>3.1498613000000002E-2</v>
+      </c>
+      <c r="G6" s="51">
+        <v>0.24493693999999999</v>
+      </c>
+      <c r="H6" s="5">
+        <v>217</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="J6" s="5">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K6" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>5.6909999999999998</v>
+      </c>
+      <c r="C7" s="51">
+        <v>2.8426304889999998</v>
+      </c>
+      <c r="D7" s="51">
+        <v>1.297982357</v>
+      </c>
+      <c r="E7" s="51">
+        <v>0.62823688499999997</v>
+      </c>
+      <c r="F7" s="51">
+        <v>0.111312536</v>
+      </c>
+      <c r="G7" s="51">
+        <v>0.18143414799999999</v>
+      </c>
+      <c r="H7" s="5">
+        <v>205</v>
+      </c>
+      <c r="I7" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.87</v>
+      </c>
+      <c r="K7" s="36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5.26</v>
+      </c>
+      <c r="C8" s="51">
+        <v>2.6780350589999999</v>
+      </c>
+      <c r="D8" s="51">
+        <v>1.2056830009999999</v>
+      </c>
+      <c r="E8" s="51">
+        <v>0.52473931600000001</v>
+      </c>
+      <c r="F8" s="51">
+        <v>8.8962947000000001E-2</v>
+      </c>
+      <c r="G8" s="51">
+        <v>0.14514497700000001</v>
+      </c>
+      <c r="H8" s="5">
+        <v>234</v>
+      </c>
+      <c r="I8" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="K8" s="36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3">
+        <v>7.2439999999999998</v>
+      </c>
+      <c r="C9" s="51">
+        <v>3.0539264519999998</v>
+      </c>
+      <c r="D9" s="51">
+        <v>1.25686728</v>
+      </c>
+      <c r="E9" s="51">
+        <v>0.80109618100000002</v>
+      </c>
+      <c r="F9" s="51">
+        <v>0.143091253</v>
+      </c>
+      <c r="G9" s="51">
+        <v>0.219020838</v>
+      </c>
+      <c r="H9" s="5">
+        <v>256</v>
+      </c>
+      <c r="I9" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="J9" s="5">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="K9" s="36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>6.8129999999999997</v>
+      </c>
+      <c r="C10" s="51">
+        <v>2.802097689</v>
+      </c>
+      <c r="D10" s="51">
+        <v>1.271869846</v>
+      </c>
+      <c r="E10" s="51">
+        <v>0.71991412600000004</v>
+      </c>
+      <c r="F10" s="51">
+        <v>0.131122293</v>
+      </c>
+      <c r="G10" s="51">
+        <v>0.2181767</v>
+      </c>
+      <c r="H10" s="5">
+        <v>258</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1.45</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3">
+        <v>10.91</v>
+      </c>
+      <c r="C11" s="51">
+        <v>3.8313944470000001</v>
+      </c>
+      <c r="D11" s="51">
+        <v>1.266508312</v>
+      </c>
+      <c r="E11" s="51">
+        <v>1.542485337</v>
+      </c>
+      <c r="F11" s="51">
+        <v>0.46597889100000001</v>
+      </c>
+      <c r="G11" s="51">
+        <v>0.20833141199999999</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7">
+        <v>5.0579999999999998</v>
+      </c>
+      <c r="C12" s="52">
+        <v>2.100406328</v>
+      </c>
+      <c r="D12" s="52">
+        <v>1.1924919970000001</v>
+      </c>
+      <c r="E12" s="52">
+        <v>0.36610933299999998</v>
+      </c>
+      <c r="F12" s="52">
+        <v>5.7670434999999999E-2</v>
+      </c>
+      <c r="G12" s="52">
+        <v>0.14365261700000001</v>
+      </c>
+      <c r="H12" s="8">
+        <v>296</v>
+      </c>
+      <c r="I12" s="8">
+        <v>4.7</v>
+      </c>
+      <c r="J12" s="8">
+        <v>1.37</v>
+      </c>
+      <c r="K12" s="38" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="54" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="50" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="50" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="50" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="50" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="50" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A56B11-718E-4AE7-9179-87FD14790215}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -3429,184 +4289,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="17">
+        <v>353</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="29">
+        <v>4.2620392137853598</v>
+      </c>
+      <c r="E2" s="29">
+        <v>352.56527253677598</v>
+      </c>
+      <c r="F2" s="30">
+        <v>0.59551488293251775</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="17">
+        <v>353</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="29">
+        <v>1.8475515119346599</v>
+      </c>
+      <c r="E3" s="29">
+        <v>277.889460280744</v>
+      </c>
+      <c r="F3" s="30">
+        <v>0.89028944637014551</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="17">
+        <v>353</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0.18802276820660199</v>
+      </c>
+      <c r="E4" s="29">
+        <v>133.637304682814</v>
+      </c>
+      <c r="F4" s="30">
+        <v>1.2454107763584301</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="17">
+        <v>77</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0</v>
+      </c>
+      <c r="E5" s="29">
+        <v>32.569603752361502</v>
+      </c>
+      <c r="F5" s="30">
+        <v>4.517437545870262</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="B6" s="17">
+        <v>77</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="31">
+        <v>0</v>
+      </c>
+      <c r="E6" s="29">
+        <v>0.71689651161644896</v>
+      </c>
+      <c r="F6" s="30">
+        <v>6.2271751379969018</v>
+      </c>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="B7" s="17">
         <v>77</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="18">
+      <c r="C7" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0</v>
+      </c>
+      <c r="E7" s="29">
+        <v>1.1515346814690299</v>
+      </c>
+      <c r="F7" s="30">
+        <v>2.50109746018421</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="18">
         <v>353</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="30">
-        <v>4.2620392137853598</v>
-      </c>
-      <c r="E2" s="30">
-        <v>352.56527253677598</v>
-      </c>
-      <c r="F2" s="31">
-        <v>0.59551488293251775</v>
-      </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-    </row>
-    <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="18">
-        <v>353</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="30">
-        <v>1.8475515119346599</v>
-      </c>
-      <c r="E3" s="30">
-        <v>277.889460280744</v>
-      </c>
-      <c r="F3" s="31">
-        <v>0.89028944637014551</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="18">
-        <v>353</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="30">
-        <v>0.18802276820660199</v>
-      </c>
-      <c r="E4" s="30">
-        <v>133.637304682814</v>
-      </c>
-      <c r="F4" s="31">
-        <v>1.2454107763584301</v>
-      </c>
-      <c r="G4" s="17"/>
-      <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="18">
-        <v>77</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="32">
-        <v>0</v>
-      </c>
-      <c r="E5" s="30">
-        <v>32.569603752361502</v>
-      </c>
-      <c r="F5" s="31">
-        <v>4.517437545870262</v>
-      </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="28" t="s">
+      <c r="C8" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="18">
-        <v>77</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="32">
-        <v>0</v>
-      </c>
-      <c r="E6" s="30">
-        <v>0.71689651161644896</v>
-      </c>
-      <c r="F6" s="31">
-        <v>6.2271751379969018</v>
-      </c>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="18">
-        <v>77</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="32">
-        <v>0</v>
-      </c>
-      <c r="E7" s="30">
-        <v>1.1515346814690299</v>
-      </c>
-      <c r="F7" s="31">
-        <v>2.50109746018421</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="19">
-        <v>353</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="34">
+      <c r="D8" s="33">
         <v>0.17249999999999999</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="33">
         <v>104</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="34">
         <v>2.0824385081391821</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="25" t="s">
-        <v>105</v>
+      <c r="A9" s="24" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -3614,7 +4474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0540222E-1C41-4607-9C02-82045FD0625E}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -3628,21 +4488,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="2">
@@ -3657,7 +4517,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="2">
@@ -3672,7 +4532,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="2">
@@ -3687,7 +4547,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="36" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="2">
@@ -3702,7 +4562,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="2">
@@ -3717,7 +4577,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="2">
@@ -3732,7 +4592,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="2">
@@ -3747,7 +4607,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="2">
@@ -3762,16 +4622,16 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>3</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>399</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <f t="shared" si="2"/>
         <v>108</v>
       </c>
@@ -3795,22 +4655,22 @@
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="9"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E923F64B-CDC3-48DA-AA7A-E7DEEA8E7B85}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3819,175 +4679,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="A1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.35">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="22" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="17">
+        <v>3.823</v>
+      </c>
+      <c r="C4" s="17">
+        <v>2.7989999999999999</v>
+      </c>
+      <c r="D4" s="17">
+        <v>3.722</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="17">
+        <v>4.2060000000000004</v>
+      </c>
+      <c r="C5" s="17">
+        <v>3.06</v>
+      </c>
+      <c r="D5" s="17">
+        <v>3.9249999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="37">
+        <v>0.03</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="18">
-        <v>3.823</v>
-      </c>
-      <c r="C4" s="18">
-        <v>2.7989999999999999</v>
-      </c>
-      <c r="D4" s="18">
-        <v>3.722</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="18">
-        <v>4.2060000000000004</v>
-      </c>
-      <c r="C5" s="18">
-        <v>3.06</v>
-      </c>
-      <c r="D5" s="18">
-        <v>3.9249999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="24" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+    </row>
+    <row r="8" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="17">
+        <v>3.66</v>
+      </c>
+      <c r="C8" s="17">
+        <v>1</v>
+      </c>
+      <c r="D8" s="17">
+        <v>2.528</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="17">
+        <v>4</v>
+      </c>
+      <c r="C9" s="17">
+        <v>1</v>
+      </c>
+      <c r="D9" s="17">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B10" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="38">
-        <v>0.03</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-    </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="18">
-        <v>3.66</v>
-      </c>
-      <c r="C8" s="18">
-        <v>1</v>
-      </c>
-      <c r="D8" s="18">
-        <v>2.528</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="18">
-        <v>4</v>
-      </c>
-      <c r="C9" s="18">
-        <v>1</v>
-      </c>
-      <c r="D9" s="18">
-        <v>2.86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>0.84</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="37" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11" s="18">
+        <v>90</v>
+      </c>
+      <c r="B11" s="17">
         <v>4.4800000000000004</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>3.6</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>0.73</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="18">
+        <v>91</v>
+      </c>
+      <c r="B12" s="17">
         <v>0.21</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>0.01</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>0.15</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="19">
+      <c r="A13" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="18">
         <v>22.9</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="18">
         <v>2.8</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="18">
         <v>16.2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="25" t="s">
-        <v>101</v>
+      <c r="A14" s="24" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="25"/>
+      <c r="A15" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3998,12 +4858,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3D7D9E-1D72-47A2-A573-6B5699B9C522}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4015,25 +4875,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4048,16 +4908,16 @@
         <v>66</v>
       </c>
       <c r="D2" s="2">
-        <v>77</v>
-      </c>
-      <c r="E2" s="2">
-        <v>6.9189234649999998</v>
+        <v>57</v>
+      </c>
+      <c r="E2" s="51">
+        <v>8.5750940338108705</v>
       </c>
       <c r="F2" s="2">
-        <v>76</v>
-      </c>
-      <c r="G2" s="14">
-        <v>6.2400000000000002E-10</v>
+        <v>56</v>
+      </c>
+      <c r="G2" s="13">
+        <v>4.4200000000000001E-12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -4071,16 +4931,16 @@
         <v>66</v>
       </c>
       <c r="D3" s="2">
-        <v>77</v>
-      </c>
-      <c r="E3" s="2">
-        <v>6.0854249930000002</v>
+        <v>65</v>
+      </c>
+      <c r="E3" s="51">
+        <v>7.6276750054811302</v>
       </c>
       <c r="F3" s="2">
-        <v>76</v>
-      </c>
-      <c r="G3" s="14">
-        <v>2.1900000000000001E-8</v>
+        <v>64</v>
+      </c>
+      <c r="G3" s="13">
+        <v>7.3099999999999998E-11</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -4094,16 +4954,16 @@
         <v>66</v>
       </c>
       <c r="D4" s="2">
-        <v>77</v>
-      </c>
-      <c r="E4" s="2">
-        <v>5.7573114350000001</v>
+        <v>58</v>
+      </c>
+      <c r="E4" s="51">
+        <v>7.5317065962948604</v>
       </c>
       <c r="F4" s="2">
-        <v>76</v>
-      </c>
-      <c r="G4" s="14">
-        <v>8.5599999999999999E-8</v>
+        <v>57</v>
+      </c>
+      <c r="G4" s="13">
+        <v>2.0700000000000001E-10</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -4117,16 +4977,16 @@
         <v>66</v>
       </c>
       <c r="D5" s="2">
-        <v>77</v>
-      </c>
-      <c r="E5" s="2">
-        <v>5.3150029769999998</v>
+        <v>53</v>
+      </c>
+      <c r="E5" s="51">
+        <v>7.5281357802584203</v>
       </c>
       <c r="F5" s="2">
-        <v>76</v>
-      </c>
-      <c r="G5" s="14">
-        <v>5.1600000000000001E-7</v>
+        <v>52</v>
+      </c>
+      <c r="G5" s="13">
+        <v>3.5600000000000001E-10</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -4140,16 +5000,16 @@
         <v>66</v>
       </c>
       <c r="D6" s="2">
-        <v>77</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.880580589</v>
+        <v>51</v>
+      </c>
+      <c r="E6" s="51">
+        <v>7.0371757052109398</v>
       </c>
       <c r="F6" s="2">
-        <v>76</v>
-      </c>
-      <c r="G6" s="13">
-        <v>3.1899999999999998E-2</v>
+        <v>50</v>
+      </c>
+      <c r="G6" s="12">
+        <v>2.6200000000000001E-9</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -4163,16 +5023,16 @@
         <v>66</v>
       </c>
       <c r="D7" s="2">
-        <v>77</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.1857208669999999</v>
+        <v>54</v>
+      </c>
+      <c r="E7" s="51">
+        <v>6.6373909974604999</v>
       </c>
       <c r="F7" s="2">
-        <v>76</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.12</v>
+        <v>53</v>
+      </c>
+      <c r="G7" s="12">
+        <v>8.6399999999999999E-9</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -4186,16 +5046,16 @@
         <v>66</v>
       </c>
       <c r="D8" s="2">
-        <v>77</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.485316162</v>
+        <v>68</v>
+      </c>
+      <c r="E8" s="51">
+        <v>5.5046890701200999</v>
       </c>
       <c r="F8" s="2">
-        <v>76</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.314</v>
+        <v>67</v>
+      </c>
+      <c r="G8" s="12">
+        <v>3.15E-7</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -4209,16 +5069,16 @@
         <v>66</v>
       </c>
       <c r="D9" s="2">
-        <v>77</v>
-      </c>
-      <c r="E9" s="2">
-        <v>-6.2599383999999994E-2</v>
+        <v>24</v>
+      </c>
+      <c r="E9" s="51">
+        <v>6.7666243483050197</v>
       </c>
       <c r="F9" s="2">
-        <v>76</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.52500000000000002</v>
+        <v>23</v>
+      </c>
+      <c r="G9" s="12">
+        <v>3.34E-7</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -4232,16 +5092,16 @@
         <v>66</v>
       </c>
       <c r="D10" s="2">
-        <v>77</v>
-      </c>
-      <c r="E10" s="2">
-        <v>-3.2760929079999999</v>
+        <v>31</v>
+      </c>
+      <c r="E10" s="51">
+        <v>5.7454015295673599</v>
       </c>
       <c r="F10" s="2">
-        <v>76</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0.999</v>
+        <v>30</v>
+      </c>
+      <c r="G10" s="12">
+        <v>1.42E-6</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -4255,39 +5115,39 @@
         <v>66</v>
       </c>
       <c r="D11" s="2">
-        <v>77</v>
-      </c>
-      <c r="E11" s="2">
-        <v>-4.5582237729999999</v>
+        <v>21</v>
+      </c>
+      <c r="E11" s="51">
+        <v>4.3823779823996798</v>
       </c>
       <c r="F11" s="2">
-        <v>76</v>
-      </c>
-      <c r="G11" s="2">
+        <v>20</v>
+      </c>
+      <c r="G11" s="12">
+        <v>1.44E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="7">
-        <v>77</v>
-      </c>
-      <c r="E12" s="7">
-        <v>-6.1089230160000003</v>
-      </c>
-      <c r="F12" s="7">
-        <v>76</v>
-      </c>
-      <c r="G12" s="7">
-        <v>1</v>
+      <c r="D12" s="6">
+        <v>35</v>
+      </c>
+      <c r="E12" s="52">
+        <v>2.9622916436154201</v>
+      </c>
+      <c r="F12" s="6">
+        <v>34</v>
+      </c>
+      <c r="G12" s="53">
+        <v>2.7699999999999999E-3</v>
       </c>
     </row>
   </sheetData>
@@ -4295,7 +5155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DED17F3-BA40-46B4-BCE1-E4A263638908}">
   <dimension ref="A1:H34"/>
   <sheetViews>
@@ -4310,28 +5170,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4357,7 +5217,7 @@
       <c r="G2" s="2">
         <v>-1.2011057836255601</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <v>1.54E-11</v>
       </c>
     </row>
@@ -4383,7 +5243,7 @@
       <c r="G3" s="2">
         <v>-0.63306377353495402</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <v>2.0199999999999999E-8</v>
       </c>
     </row>
@@ -4409,7 +5269,7 @@
       <c r="G4" s="2">
         <v>-0.52203757454775102</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="12">
         <v>8.2600000000000001E-7</v>
       </c>
     </row>
@@ -4435,7 +5295,7 @@
       <c r="G5" s="2">
         <v>-0.52391909650755797</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>2.17E-6</v>
       </c>
     </row>
@@ -4461,7 +5321,7 @@
       <c r="G6" s="2">
         <v>-0.360841367332152</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="12">
         <v>3.54E-5</v>
       </c>
     </row>
@@ -4487,7 +5347,7 @@
       <c r="G7" s="2">
         <v>-0.35151696906635899</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>9.87E-5</v>
       </c>
     </row>
@@ -4513,7 +5373,7 @@
       <c r="G8" s="2">
         <v>-0.238591627640655</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <v>2.23E-4</v>
       </c>
     </row>
@@ -4539,7 +5399,7 @@
       <c r="G9" s="2">
         <v>-0.37538738013459499</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <v>2.0799999999999998E-3</v>
       </c>
     </row>
@@ -4565,7 +5425,7 @@
       <c r="G10" s="2">
         <v>1.2891365106499799</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <v>2.64E-3</v>
       </c>
     </row>
@@ -4591,7 +5451,7 @@
       <c r="G11" s="2">
         <v>1.2666747585428599</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <v>0.04</v>
       </c>
     </row>
@@ -4617,7 +5477,7 @@
       <c r="G12" s="2">
         <v>-1.7346000171776701E-2</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="13">
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
@@ -4643,7 +5503,7 @@
       <c r="G13" s="2">
         <v>1.55981448144787</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="13">
         <v>4.1799999999999997E-2</v>
       </c>
     </row>
@@ -5168,28 +6028,28 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <v>0</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>1.2483551870117401E-2</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <v>-0.42214093021975402</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="6">
         <v>0.44710803395998899</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="6">
         <v>0.997</v>
       </c>
     </row>
@@ -5198,11 +6058,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0408A5-29FF-44CD-B26B-942799845A00}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:I13"/>
     </sheetView>
   </sheetViews>
@@ -5216,10 +6076,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
+      <c r="A1" s="42"/>
+      <c r="B1" s="42"/>
       <c r="C1" s="49" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
@@ -5229,40 +6089,40 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="41" t="s">
         <v>109</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="I2" s="44" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>110</v>
+      <c r="B3" s="39" t="s">
+        <v>102</v>
       </c>
       <c r="C3" s="3">
         <v>27.330568912155499</v>
@@ -5270,27 +6130,27 @@
       <c r="D3" s="3">
         <v>0.489440405580716</v>
       </c>
-      <c r="E3" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="H3" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="I3" s="43" t="s">
-        <v>110</v>
+      <c r="E3" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="46" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="3">
@@ -5319,7 +6179,7 @@
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="46" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="3">
@@ -5334,13 +6194,13 @@
       <c r="F5" s="3">
         <v>1.1933861219234201</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="47">
         <v>0.15003046565873099</v>
       </c>
-      <c r="H5" s="51">
+      <c r="H5" s="47">
         <v>0.199288238405298</v>
       </c>
-      <c r="I5" s="51">
+      <c r="I5" s="47">
         <v>1.0304139215994299</v>
       </c>
     </row>
@@ -5348,8 +6208,8 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="50" t="s">
-        <v>119</v>
+      <c r="B6" s="46" t="s">
+        <v>111</v>
       </c>
       <c r="C6" s="3">
         <v>2.6799754589995599</v>
@@ -5363,13 +6223,13 @@
       <c r="F6" s="3">
         <v>24.604014769609101</v>
       </c>
-      <c r="G6" s="51">
+      <c r="G6" s="47">
         <v>3.8030301536233901</v>
       </c>
-      <c r="H6" s="51">
+      <c r="H6" s="47">
         <v>2.7726652663543998</v>
       </c>
-      <c r="I6" s="51">
+      <c r="I6" s="47">
         <v>4.4211878771971902</v>
       </c>
     </row>
@@ -5377,8 +6237,8 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="42" t="s">
-        <v>110</v>
+      <c r="B7" s="39" t="s">
+        <v>102</v>
       </c>
       <c r="C7" s="3">
         <v>12.529017818742799</v>
@@ -5386,28 +6246,28 @@
       <c r="D7" s="3">
         <v>0.21644905946687801</v>
       </c>
-      <c r="E7" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="F7" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="H7" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="I7" s="43" t="s">
-        <v>110</v>
+      <c r="E7" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="40" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="42" t="s">
-        <v>110</v>
+      <c r="B8" s="39" t="s">
+        <v>102</v>
       </c>
       <c r="C8" s="3">
         <v>20.008337061990201</v>
@@ -5415,28 +6275,28 @@
       <c r="D8" s="3">
         <v>1.1078012944945601</v>
       </c>
-      <c r="E8" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="I8" s="43" t="s">
-        <v>110</v>
+      <c r="E8" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="42" t="s">
-        <v>110</v>
+      <c r="B9" s="39" t="s">
+        <v>102</v>
       </c>
       <c r="C9" s="3">
         <v>2.5194832031572298</v>
@@ -5444,28 +6304,28 @@
       <c r="D9" s="3">
         <v>6.7848198143704699E-2</v>
       </c>
-      <c r="E9" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="F9" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="G9" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="H9" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="I9" s="43" t="s">
-        <v>110</v>
+      <c r="E9" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="40" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="42" t="s">
-        <v>110</v>
+      <c r="B10" s="39" t="s">
+        <v>102</v>
       </c>
       <c r="C10" s="3">
         <v>1.7357985383183401</v>
@@ -5473,28 +6333,28 @@
       <c r="D10" s="3">
         <v>0.111496865218578</v>
       </c>
-      <c r="E10" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="G10" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="H10" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="I10" s="43" t="s">
-        <v>110</v>
+      <c r="E10" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="42" t="s">
-        <v>110</v>
+      <c r="B11" s="39" t="s">
+        <v>102</v>
       </c>
       <c r="C11" s="3">
         <v>8.9410544110129493</v>
@@ -5502,78 +6362,78 @@
       <c r="D11" s="3">
         <v>3.2475923989966599E-2</v>
       </c>
-      <c r="E11" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="G11" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="H11" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="I11" s="43" t="s">
-        <v>110</v>
+      <c r="E11" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="52">
+      <c r="B12" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="3">
         <v>12.994924080443001</v>
       </c>
-      <c r="D12" s="52">
+      <c r="D12" s="3">
         <v>0.69231273379018798</v>
       </c>
-      <c r="E12" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="G12" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="H12" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="I12" s="43" t="s">
-        <v>110</v>
+      <c r="E12" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" s="40" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="B13" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="7">
         <v>2.3007447015073699</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>9.8601768533661302E-2</v>
       </c>
-      <c r="E13" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="F13" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="G13" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="H13" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" s="47" t="s">
-        <v>110</v>
+      <c r="E13" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>